<commit_message>
export table finished,element position optimization >>>>(roger part only on price tier>test_cloud_intergration)
</commit_message>
<xml_diff>
--- a/ClassroomAutoTestServer/price tier/xlsx/sign in.xlsx
+++ b/ClassroomAutoTestServer/price tier/xlsx/sign in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liouki\Viewsonic-AutoTest\ClassroomAutoTestServer\price tier\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF4D20C-F7DD-4F10-BEDC-CF9DA0D05ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831257C2-7E73-475B-A276-70BFA4E76B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{301211D1-6A8D-41C4-B6F5-813360E33792}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="85">
   <si>
     <t>點擊登入按鈕</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,53 +121,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>測試about</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>點擊about</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>測試qrcode_share</t>
   </si>
   <si>
     <t>點擊</t>
   </si>
   <si>
-    <t>顯示about視窗</t>
-  </si>
-  <si>
-    <t>顯示</t>
-  </si>
-  <si>
     <t>點擊一般設定</t>
   </si>
   <si>
     <t>截圖比對</t>
   </si>
   <si>
-    <t>關閉setting視窗</t>
-  </si>
-  <si>
     <t>點擊"使用qrcode分享檔案"</t>
   </si>
   <si>
     <t>點擊maintoolbar內file management</t>
   </si>
   <si>
-    <t>顯示file managment視窗</t>
-  </si>
-  <si>
-    <t>顯示myviewboard收費方案視窗</t>
-  </si>
-  <si>
-    <t>點擊myviewboard收費方案視窗內取消</t>
-  </si>
-  <si>
-    <t>顯示myviewboard收費方案視窗關閉</t>
-  </si>
-  <si>
     <t>測試user_profile</t>
   </si>
   <si>
@@ -199,6 +170,147 @@
   </si>
   <si>
     <t>測試項目</t>
+  </si>
+  <si>
+    <t>顯示file management視窗</t>
+  </si>
+  <si>
+    <t>顯示myViewBoard收費方案視窗</t>
+  </si>
+  <si>
+    <t>點擊myViewBoard收費方案視窗內取消</t>
+  </si>
+  <si>
+    <t>顯示myViewBoard收費方案視窗關閉</t>
+  </si>
+  <si>
+    <t>顯示shapes,lines,tables視窗</t>
+  </si>
+  <si>
+    <t>點擊上一頁按鈕(消除tool tip)</t>
+  </si>
+  <si>
+    <t>測試shapes_lines</t>
+  </si>
+  <si>
+    <t>點擊lines</t>
+  </si>
+  <si>
+    <t>顯示lines視窗</t>
+  </si>
+  <si>
+    <t>測試shapes_3Dshapes</t>
+  </si>
+  <si>
+    <t>點擊3Dshapes</t>
+  </si>
+  <si>
+    <t>顯示3Dshapes視窗</t>
+  </si>
+  <si>
+    <t>測試test_shapes_tables</t>
+  </si>
+  <si>
+    <t>點擊tables</t>
+  </si>
+  <si>
+    <t>顯示tables視窗</t>
+  </si>
+  <si>
+    <t>點擊shapes,lines,tables視窗內X</t>
+  </si>
+  <si>
+    <t>顯示shapes,lines,tables視窗關閉</t>
+  </si>
+  <si>
+    <t>測試text</t>
+  </si>
+  <si>
+    <t>點擊main tool bar內text</t>
+  </si>
+  <si>
+    <t>顯示text tooltip</t>
+  </si>
+  <si>
+    <t>點擊白板一處讓text功能顯示出來</t>
+  </si>
+  <si>
+    <t>顯示文字編輯器</t>
+  </si>
+  <si>
+    <t>點擊文字編輯器內X</t>
+  </si>
+  <si>
+    <t>顯示文字編輯器關閉</t>
+  </si>
+  <si>
+    <t>測試background</t>
+  </si>
+  <si>
+    <t>顯示background視窗</t>
+  </si>
+  <si>
+    <t>點擊main tool bar內background</t>
+  </si>
+  <si>
+    <t>測試background_original</t>
+  </si>
+  <si>
+    <t>雙擊main tool bar內shapes,lines,tables</t>
+  </si>
+  <si>
+    <t>點擊background視窗內Originals</t>
+  </si>
+  <si>
+    <t>顯示Originals視窗</t>
+  </si>
+  <si>
+    <t>顯示Originals視窗關閉</t>
+  </si>
+  <si>
+    <t>測試background_googledrive</t>
+  </si>
+  <si>
+    <t>顯示background視窗關閉</t>
+  </si>
+  <si>
+    <t>點擊background視窗內Google雲端硬碟</t>
+  </si>
+  <si>
+    <t>顯示Google雲端硬碟視窗</t>
+  </si>
+  <si>
+    <t>顯示Google雲端硬碟視窗關閉</t>
+  </si>
+  <si>
+    <t>測試background_image_search</t>
+  </si>
+  <si>
+    <t>顯示background_image_search視窗</t>
+  </si>
+  <si>
+    <t>點擊background視窗內圖片搜尋</t>
+  </si>
+  <si>
+    <t>顯示background_image_search視窗消除打字時候後面一閃一閃的小豎線</t>
+  </si>
+  <si>
+    <t>顯示圖片搜尋視窗關閉</t>
+  </si>
+  <si>
+    <t>測試background_color</t>
+  </si>
+  <si>
+    <t>顯示background_color視窗</t>
+  </si>
+  <si>
+    <t>點擊background視窗內底色</t>
+  </si>
+  <si>
+    <t>顯示background_color視窗關閉</t>
+  </si>
+  <si>
+    <t>點擊X</t>
   </si>
 </sst>
 </file>
@@ -565,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86006B1-E128-4347-AFEC-1926B734B60C}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -580,7 +692,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -591,10 +703,10 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -602,7 +714,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -613,7 +725,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -624,7 +736,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -635,7 +747,7 @@
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -646,7 +758,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -668,10 +780,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -679,18 +791,18 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -712,7 +824,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
@@ -723,18 +835,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -748,289 +860,510 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>